<commit_message>
Updated the MDNL data for SSC to get rid of non-numeric characters
</commit_message>
<xml_diff>
--- a/usgs-sediment/harpeth_river_USGS.xlsx
+++ b/usgs-sediment/harpeth_river_USGS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moyoa\Documents\GitHub\MATLAB_Functions\usgs-sediment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C04656-3FBE-4D3F-8B60-6E914B768D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EBC1E6-0725-4DD1-ACB6-D47D69BACFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-4392" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{B5D21F95-566D-44EE-AF36-F6105D2006C2}"/>
+    <workbookView xWindow="-23148" yWindow="-4392" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="8" xr2:uid="{B5D21F95-566D-44EE-AF36-F6105D2006C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Variable_Info" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5389" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5388" uniqueCount="240">
   <si>
     <t>agency_cd</t>
   </si>
@@ -762,17 +762,15 @@
   <si>
     <t>S</t>
   </si>
-  <si>
-    <t>&lt;0.5</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mmm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="165" formatCode="dd/mmm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -811,12 +809,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3467,8 +3468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7818C5EF-33CE-424D-A715-17D27A86FEE1}">
   <dimension ref="A1:AS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4540,8 +4542,8 @@
   <dimension ref="A1:I2130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C2130"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40782,9 +40784,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71537EC4-1369-4D3D-9549-8752C3492659}">
   <dimension ref="A1:AS195"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40949,9 +40951,10 @@
       <c r="E2" t="s">
         <v>239</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="7">
         <v>11</v>
       </c>
+      <c r="G2" s="7"/>
       <c r="Y2">
         <v>900</v>
       </c>
@@ -40972,10 +40975,10 @@
       <c r="E3" t="s">
         <v>239</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="7">
         <v>305</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="7">
         <v>865</v>
       </c>
       <c r="Y3">
@@ -41007,10 +41010,10 @@
       <c r="E4" t="s">
         <v>239</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <v>423</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>865</v>
       </c>
       <c r="Y4">
@@ -41042,10 +41045,10 @@
       <c r="E5" t="s">
         <v>239</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>428</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>865</v>
       </c>
       <c r="Y5">
@@ -41077,10 +41080,10 @@
       <c r="E6" t="s">
         <v>239</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7">
         <v>14</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="7">
         <v>122</v>
       </c>
       <c r="Y6">
@@ -41103,10 +41106,10 @@
       <c r="E7" t="s">
         <v>239</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="7">
         <v>16</v>
       </c>
       <c r="Y7">
@@ -41129,10 +41132,10 @@
       <c r="E8" t="s">
         <v>239</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="7">
         <v>16</v>
       </c>
       <c r="Y8">
@@ -41155,10 +41158,10 @@
       <c r="E9" t="s">
         <v>239</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7">
         <v>3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="7">
         <v>16</v>
       </c>
       <c r="Y9">
@@ -41181,10 +41184,10 @@
       <c r="E10" t="s">
         <v>239</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="7">
         <v>5</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7">
         <v>16</v>
       </c>
       <c r="Y10">
@@ -41207,10 +41210,10 @@
       <c r="E11" t="s">
         <v>239</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="7">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="7">
         <v>16</v>
       </c>
       <c r="Y11">
@@ -41233,10 +41236,10 @@
       <c r="E12" t="s">
         <v>239</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <v>7</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="7">
         <v>60</v>
       </c>
       <c r="Y12">
@@ -41259,10 +41262,10 @@
       <c r="E13" t="s">
         <v>239</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>6</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="7">
         <v>16</v>
       </c>
       <c r="Y13">
@@ -41285,10 +41288,10 @@
       <c r="E14" t="s">
         <v>239</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>13</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>61</v>
       </c>
       <c r="Y14">
@@ -41311,10 +41314,10 @@
       <c r="E15" t="s">
         <v>239</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="7">
         <v>269</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <v>141</v>
       </c>
       <c r="Y15">
@@ -41337,10 +41340,10 @@
       <c r="E16" t="s">
         <v>239</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="7">
         <v>212</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="7">
         <v>59</v>
       </c>
       <c r="Y16">
@@ -41363,10 +41366,10 @@
       <c r="E17" t="s">
         <v>239</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="7">
         <v>19</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="7">
         <v>5.8</v>
       </c>
       <c r="Y17">
@@ -41389,10 +41392,10 @@
       <c r="E18" t="s">
         <v>239</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="7">
         <v>14</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="7">
         <v>2.2999999999999998</v>
       </c>
       <c r="Y18">
@@ -41415,10 +41418,10 @@
       <c r="E19" t="s">
         <v>239</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="7">
         <v>11</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="7">
         <v>1.1000000000000001</v>
       </c>
       <c r="Y19">
@@ -41441,10 +41444,10 @@
       <c r="E20" t="s">
         <v>239</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="7">
         <v>54</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="7">
         <v>8</v>
       </c>
       <c r="Y20">
@@ -41467,10 +41470,10 @@
       <c r="E21" t="s">
         <v>239</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="7">
         <v>54</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="7">
         <v>12</v>
       </c>
       <c r="Y21">
@@ -41493,10 +41496,10 @@
       <c r="E22" t="s">
         <v>239</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="7">
         <v>89</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="7">
         <v>12</v>
       </c>
       <c r="Y22">
@@ -41519,10 +41522,10 @@
       <c r="E23" t="s">
         <v>239</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="7">
         <v>63</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="7">
         <v>36</v>
       </c>
       <c r="Y23">
@@ -41545,10 +41548,10 @@
       <c r="E24" t="s">
         <v>239</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="7">
         <v>56</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="7">
         <v>1.4</v>
       </c>
       <c r="H24">
@@ -41574,10 +41577,10 @@
       <c r="E25" t="s">
         <v>239</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="7">
         <v>6</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="7">
         <v>55</v>
       </c>
       <c r="H25">
@@ -41603,10 +41606,10 @@
       <c r="E26" t="s">
         <v>239</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="7">
         <v>118</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="7">
         <v>334</v>
       </c>
       <c r="H26">
@@ -41632,10 +41635,10 @@
       <c r="E27" t="s">
         <v>239</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="7">
         <v>140</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="7">
         <v>790</v>
       </c>
       <c r="H27">
@@ -41661,10 +41664,10 @@
       <c r="E28" t="s">
         <v>239</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="7">
         <v>115</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="7">
         <v>790</v>
       </c>
       <c r="H28">
@@ -41690,10 +41693,10 @@
       <c r="E29" t="s">
         <v>239</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="7">
         <v>35</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="7">
         <v>712</v>
       </c>
       <c r="H29">
@@ -41719,10 +41722,10 @@
       <c r="E30" t="s">
         <v>239</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="7">
         <v>51</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="7">
         <v>712</v>
       </c>
       <c r="H30">
@@ -41748,10 +41751,10 @@
       <c r="E31" t="s">
         <v>239</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="7">
         <v>39</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="7">
         <v>170</v>
       </c>
       <c r="H31">
@@ -41777,10 +41780,10 @@
       <c r="E32" t="s">
         <v>239</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="7">
         <v>21</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="7">
         <v>170</v>
       </c>
       <c r="H32">
@@ -41806,10 +41809,10 @@
       <c r="E33" t="s">
         <v>239</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="7">
         <v>77</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="7">
         <v>1260</v>
       </c>
       <c r="H33">
@@ -41838,10 +41841,10 @@
       <c r="E34" t="s">
         <v>239</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="7">
         <v>204</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="7">
         <v>1260</v>
       </c>
       <c r="H34">
@@ -41870,10 +41873,10 @@
       <c r="E35" t="s">
         <v>239</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="7">
         <v>70</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="7">
         <v>690</v>
       </c>
       <c r="H35">
@@ -41902,10 +41905,10 @@
       <c r="E36" t="s">
         <v>239</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="7">
         <v>58</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="7">
         <v>690</v>
       </c>
       <c r="H36">
@@ -41934,10 +41937,10 @@
       <c r="E37" t="s">
         <v>239</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="7">
         <v>34</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="7">
         <v>223</v>
       </c>
       <c r="H37">
@@ -41966,10 +41969,10 @@
       <c r="E38" t="s">
         <v>239</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="7">
         <v>92</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="7">
         <v>156</v>
       </c>
       <c r="H38">
@@ -41998,10 +42001,10 @@
       <c r="E39" t="s">
         <v>239</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="7">
         <v>211</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="7">
         <v>53</v>
       </c>
       <c r="H39">
@@ -42030,10 +42033,10 @@
       <c r="E40" t="s">
         <v>239</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="7">
         <v>274</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="7">
         <v>2.9</v>
       </c>
       <c r="H40">
@@ -42059,10 +42062,10 @@
       <c r="E41" t="s">
         <v>239</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="7">
         <v>18</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="7">
         <v>0.46</v>
       </c>
       <c r="H41">
@@ -42088,10 +42091,10 @@
       <c r="E42" t="s">
         <v>239</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="7">
         <v>88</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="7">
         <v>3.8</v>
       </c>
       <c r="H42">
@@ -42117,10 +42120,10 @@
       <c r="E43" t="s">
         <v>239</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="7">
         <v>97</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="7">
         <v>3.8</v>
       </c>
       <c r="H43">
@@ -42146,10 +42149,10 @@
       <c r="E44" t="s">
         <v>239</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="7">
         <v>82</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="7">
         <v>125</v>
       </c>
       <c r="Y44">
@@ -42172,10 +42175,10 @@
       <c r="E45" t="s">
         <v>239</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="7">
         <v>632</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="7">
         <v>1280</v>
       </c>
       <c r="H45">
@@ -42198,10 +42201,10 @@
       <c r="E46" t="s">
         <v>239</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="7">
         <v>1030</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="7">
         <v>1280</v>
       </c>
       <c r="H46">
@@ -42224,10 +42227,10 @@
       <c r="E47" t="s">
         <v>239</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="7">
         <v>394</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="7">
         <v>1280</v>
       </c>
       <c r="H47">
@@ -42250,10 +42253,10 @@
       <c r="E48" t="s">
         <v>239</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="7">
         <v>252</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="7">
         <v>1280</v>
       </c>
       <c r="H48">
@@ -42276,10 +42279,10 @@
       <c r="E49" t="s">
         <v>239</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="7">
         <v>293</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="7">
         <v>1280</v>
       </c>
       <c r="H49">
@@ -42302,10 +42305,10 @@
       <c r="E50" t="s">
         <v>239</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="7">
         <v>67</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="7">
         <v>593</v>
       </c>
       <c r="H50">
@@ -42328,10 +42331,10 @@
       <c r="E51" t="s">
         <v>239</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="7">
         <v>77</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="7">
         <v>783</v>
       </c>
       <c r="H51">
@@ -42354,10 +42357,10 @@
       <c r="E52" t="s">
         <v>239</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="7">
         <v>135</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="7">
         <v>137</v>
       </c>
       <c r="H52">
@@ -42380,10 +42383,10 @@
       <c r="E53" t="s">
         <v>239</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="7">
         <v>85</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="7">
         <v>174</v>
       </c>
       <c r="H53">
@@ -42406,10 +42409,10 @@
       <c r="E54" t="s">
         <v>239</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="7">
         <v>431</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="7">
         <v>174</v>
       </c>
       <c r="H54">
@@ -42432,10 +42435,10 @@
       <c r="E55" t="s">
         <v>239</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="7">
         <v>141</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="7">
         <v>403</v>
       </c>
       <c r="H55">
@@ -42458,10 +42461,10 @@
       <c r="E56" t="s">
         <v>239</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="7">
         <v>285</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="7">
         <v>403</v>
       </c>
       <c r="H56">
@@ -42484,10 +42487,10 @@
       <c r="E57" t="s">
         <v>239</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="7">
         <v>277</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="7">
         <v>403</v>
       </c>
       <c r="H57">
@@ -42510,10 +42513,10 @@
       <c r="E58" t="s">
         <v>239</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="7">
         <v>68</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="7">
         <v>368</v>
       </c>
       <c r="H58">
@@ -42536,10 +42539,10 @@
       <c r="E59" t="s">
         <v>239</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="7">
         <v>159</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="7">
         <v>368</v>
       </c>
       <c r="H59">
@@ -42562,10 +42565,10 @@
       <c r="E60" t="s">
         <v>239</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="7">
         <v>96</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="7">
         <v>651</v>
       </c>
       <c r="H60">
@@ -42588,10 +42591,10 @@
       <c r="E61" t="s">
         <v>239</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="7">
         <v>61</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="7">
         <v>651</v>
       </c>
       <c r="H61">
@@ -42614,10 +42617,10 @@
       <c r="E62" t="s">
         <v>239</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="7">
         <v>44</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="7">
         <v>651</v>
       </c>
       <c r="H62">
@@ -42640,10 +42643,10 @@
       <c r="E63" t="s">
         <v>239</v>
       </c>
-      <c r="F63" t="s">
-        <v>240</v>
-      </c>
-      <c r="G63">
+      <c r="F63" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G63" s="7">
         <v>651</v>
       </c>
       <c r="H63">
@@ -42666,10 +42669,10 @@
       <c r="E64" t="s">
         <v>239</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="7">
         <v>63</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="7">
         <v>230</v>
       </c>
       <c r="H64">
@@ -42692,10 +42695,10 @@
       <c r="E65" t="s">
         <v>239</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="7">
         <v>80</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="7">
         <v>230</v>
       </c>
       <c r="H65">
@@ -42718,10 +42721,10 @@
       <c r="E66" t="s">
         <v>239</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="7">
         <v>25</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="7">
         <v>722</v>
       </c>
       <c r="H66">
@@ -42744,10 +42747,10 @@
       <c r="E67" t="s">
         <v>239</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="7">
         <v>367</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="7">
         <v>722</v>
       </c>
       <c r="H67">
@@ -42770,10 +42773,10 @@
       <c r="E68" t="s">
         <v>239</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="7">
         <v>401</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="7">
         <v>1080</v>
       </c>
       <c r="H68">
@@ -42796,10 +42799,10 @@
       <c r="E69" t="s">
         <v>239</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="7">
         <v>292</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="7">
         <v>1080</v>
       </c>
       <c r="H69">
@@ -42822,10 +42825,10 @@
       <c r="E70" t="s">
         <v>239</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="7">
         <v>439</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="7">
         <v>402</v>
       </c>
       <c r="H70">
@@ -42848,10 +42851,10 @@
       <c r="E71" t="s">
         <v>239</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="7">
         <v>487</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="7">
         <v>311</v>
       </c>
       <c r="H71">
@@ -42874,10 +42877,10 @@
       <c r="E72" t="s">
         <v>239</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="7">
         <v>452</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="7">
         <v>334</v>
       </c>
       <c r="H72">
@@ -42900,10 +42903,10 @@
       <c r="E73" t="s">
         <v>239</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="7">
         <v>419</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="7">
         <v>334</v>
       </c>
       <c r="H73">
@@ -42926,10 +42929,10 @@
       <c r="E74" t="s">
         <v>239</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="7">
         <v>645</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="7">
         <v>334</v>
       </c>
       <c r="H74">
@@ -42952,10 +42955,10 @@
       <c r="E75" t="s">
         <v>239</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="7">
         <v>630</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="7">
         <v>334</v>
       </c>
       <c r="H75">
@@ -42978,10 +42981,10 @@
       <c r="E76" t="s">
         <v>239</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="7">
         <v>382</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="7">
         <v>928</v>
       </c>
       <c r="H76">
@@ -43004,10 +43007,10 @@
       <c r="E77" t="s">
         <v>239</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="7">
         <v>253</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="7">
         <v>928</v>
       </c>
       <c r="H77">
@@ -43030,10 +43033,10 @@
       <c r="E78" t="s">
         <v>239</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="7">
         <v>175</v>
       </c>
-      <c r="G78">
+      <c r="G78" s="7">
         <v>928</v>
       </c>
       <c r="H78">
@@ -43056,10 +43059,10 @@
       <c r="E79" t="s">
         <v>239</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="7">
         <v>266</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="7">
         <v>201</v>
       </c>
       <c r="H79">
@@ -43082,10 +43085,10 @@
       <c r="E80" t="s">
         <v>239</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="7">
         <v>102</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="7">
         <v>432</v>
       </c>
       <c r="H80">
@@ -43108,10 +43111,10 @@
       <c r="E81" t="s">
         <v>239</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="7">
         <v>81</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="7">
         <v>432</v>
       </c>
       <c r="H81">
@@ -43134,10 +43137,10 @@
       <c r="E82" t="s">
         <v>239</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="7">
         <v>86</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="7">
         <v>432</v>
       </c>
       <c r="H82">
@@ -43160,10 +43163,10 @@
       <c r="E83" t="s">
         <v>239</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="7">
         <v>110</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="7">
         <v>432</v>
       </c>
       <c r="H83">
@@ -43189,10 +43192,10 @@
       <c r="E84" t="s">
         <v>239</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="7">
         <v>120</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="7">
         <v>432</v>
       </c>
       <c r="H84">
@@ -43218,10 +43221,10 @@
       <c r="E85" t="s">
         <v>239</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="7">
         <v>171</v>
       </c>
-      <c r="G85">
+      <c r="G85" s="7">
         <v>432</v>
       </c>
       <c r="H85">
@@ -43244,10 +43247,10 @@
       <c r="E86" t="s">
         <v>239</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="7">
         <v>169</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="7">
         <v>432</v>
       </c>
       <c r="H86">
@@ -43270,10 +43273,10 @@
       <c r="E87" t="s">
         <v>239</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="7">
         <v>249</v>
       </c>
-      <c r="G87">
+      <c r="G87" s="7">
         <v>432</v>
       </c>
       <c r="H87">
@@ -43296,10 +43299,10 @@
       <c r="E88" t="s">
         <v>239</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="7">
         <v>430</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="7">
         <v>432</v>
       </c>
       <c r="H88">
@@ -43325,10 +43328,10 @@
       <c r="E89" t="s">
         <v>239</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="7">
         <v>412</v>
       </c>
-      <c r="G89">
+      <c r="G89" s="7">
         <v>432</v>
       </c>
       <c r="H89">
@@ -43351,10 +43354,10 @@
       <c r="E90" t="s">
         <v>239</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="7">
         <v>620</v>
       </c>
-      <c r="G90">
+      <c r="G90" s="7">
         <v>432</v>
       </c>
       <c r="H90">
@@ -43377,10 +43380,10 @@
       <c r="E91" t="s">
         <v>239</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="7">
         <v>433</v>
       </c>
-      <c r="G91">
+      <c r="G91" s="7">
         <v>432</v>
       </c>
       <c r="H91">
@@ -43403,10 +43406,10 @@
       <c r="E92" t="s">
         <v>239</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="7">
         <v>363</v>
       </c>
-      <c r="G92">
+      <c r="G92" s="7">
         <v>432</v>
       </c>
       <c r="H92">
@@ -43429,10 +43432,10 @@
       <c r="E93" t="s">
         <v>239</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="7">
         <v>338</v>
       </c>
-      <c r="G93">
+      <c r="G93" s="7">
         <v>432</v>
       </c>
       <c r="H93">
@@ -43455,10 +43458,10 @@
       <c r="E94" t="s">
         <v>239</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="7">
         <v>184</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="7">
         <v>1820</v>
       </c>
       <c r="H94">
@@ -43484,10 +43487,10 @@
       <c r="E95" t="s">
         <v>239</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="7">
         <v>184</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="7">
         <v>1820</v>
       </c>
       <c r="H95">
@@ -43510,10 +43513,10 @@
       <c r="E96" t="s">
         <v>239</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="7">
         <v>165</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="7">
         <v>1820</v>
       </c>
       <c r="H96">
@@ -43539,10 +43542,10 @@
       <c r="E97" t="s">
         <v>239</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="7">
         <v>255</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="7">
         <v>1820</v>
       </c>
       <c r="H97">
@@ -43565,10 +43568,10 @@
       <c r="E98" t="s">
         <v>239</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="7">
         <v>446</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="7">
         <v>1820</v>
       </c>
       <c r="H98">
@@ -43591,10 +43594,10 @@
       <c r="E99" t="s">
         <v>239</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="7">
         <v>638</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="7">
         <v>1820</v>
       </c>
       <c r="H99">
@@ -43617,10 +43620,10 @@
       <c r="E100" t="s">
         <v>239</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="7">
         <v>402</v>
       </c>
-      <c r="G100">
+      <c r="G100" s="7">
         <v>1820</v>
       </c>
       <c r="H100">
@@ -43643,10 +43646,10 @@
       <c r="E101" t="s">
         <v>239</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="7">
         <v>237</v>
       </c>
-      <c r="G101">
+      <c r="G101" s="7">
         <v>1820</v>
       </c>
       <c r="H101">
@@ -43669,10 +43672,10 @@
       <c r="E102" t="s">
         <v>239</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="7">
         <v>91</v>
       </c>
-      <c r="G102">
+      <c r="G102" s="7">
         <v>312</v>
       </c>
       <c r="H102">
@@ -43695,10 +43698,10 @@
       <c r="E103" t="s">
         <v>239</v>
       </c>
-      <c r="F103">
+      <c r="F103" s="7">
         <v>66</v>
       </c>
-      <c r="G103">
+      <c r="G103" s="7">
         <v>312</v>
       </c>
       <c r="H103">
@@ -43721,10 +43724,10 @@
       <c r="E104" t="s">
         <v>239</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="7">
         <v>340</v>
       </c>
-      <c r="G104">
+      <c r="G104" s="7">
         <v>268</v>
       </c>
       <c r="H104">
@@ -43750,10 +43753,10 @@
       <c r="E105" t="s">
         <v>239</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="7">
         <v>19</v>
       </c>
-      <c r="G105">
+      <c r="G105" s="7">
         <v>23</v>
       </c>
       <c r="H105">
@@ -43776,10 +43779,10 @@
       <c r="E106" t="s">
         <v>239</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="7">
         <v>29</v>
       </c>
-      <c r="G106">
+      <c r="G106" s="7">
         <v>28</v>
       </c>
       <c r="H106">
@@ -43802,10 +43805,10 @@
       <c r="E107" t="s">
         <v>239</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="7">
         <v>24</v>
       </c>
-      <c r="G107">
+      <c r="G107" s="7">
         <v>27</v>
       </c>
       <c r="H107">
@@ -43828,10 +43831,10 @@
       <c r="E108" t="s">
         <v>239</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="7">
         <v>25</v>
       </c>
-      <c r="G108">
+      <c r="G108" s="7">
         <v>27</v>
       </c>
       <c r="H108">
@@ -43854,10 +43857,10 @@
       <c r="E109" t="s">
         <v>239</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="7">
         <v>44</v>
       </c>
-      <c r="G109">
+      <c r="G109" s="7">
         <v>27</v>
       </c>
       <c r="H109">
@@ -43880,10 +43883,10 @@
       <c r="E110" t="s">
         <v>239</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="7">
         <v>81</v>
       </c>
-      <c r="G110">
+      <c r="G110" s="7">
         <v>27</v>
       </c>
       <c r="H110">
@@ -43906,10 +43909,10 @@
       <c r="E111" t="s">
         <v>239</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="7">
         <v>13</v>
       </c>
-      <c r="G111">
+      <c r="G111" s="7">
         <v>2.4</v>
       </c>
       <c r="H111">
@@ -43932,10 +43935,10 @@
       <c r="E112" t="s">
         <v>239</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="7">
         <v>13</v>
       </c>
-      <c r="G112">
+      <c r="G112" s="7">
         <v>1.6</v>
       </c>
       <c r="H112">
@@ -43958,10 +43961,10 @@
       <c r="E113" t="s">
         <v>239</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="7">
         <v>39</v>
       </c>
-      <c r="G113">
+      <c r="G113" s="7">
         <v>72</v>
       </c>
       <c r="H113">
@@ -43984,10 +43987,10 @@
       <c r="E114" t="s">
         <v>239</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="7">
         <v>79</v>
       </c>
-      <c r="G114">
+      <c r="G114" s="7">
         <v>72</v>
       </c>
       <c r="H114">
@@ -44010,10 +44013,10 @@
       <c r="E115" t="s">
         <v>239</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="7">
         <v>87</v>
       </c>
-      <c r="G115">
+      <c r="G115" s="7">
         <v>72</v>
       </c>
       <c r="H115">
@@ -44036,10 +44039,10 @@
       <c r="E116" t="s">
         <v>239</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="7">
         <v>101</v>
       </c>
-      <c r="G116">
+      <c r="G116" s="7">
         <v>72</v>
       </c>
       <c r="H116">
@@ -44062,10 +44065,10 @@
       <c r="E117" t="s">
         <v>239</v>
       </c>
-      <c r="F117">
+      <c r="F117" s="7">
         <v>118</v>
       </c>
-      <c r="G117">
+      <c r="G117" s="7">
         <v>72</v>
       </c>
       <c r="H117">
@@ -44088,10 +44091,10 @@
       <c r="E118" t="s">
         <v>239</v>
       </c>
-      <c r="F118">
+      <c r="F118" s="7">
         <v>88</v>
       </c>
-      <c r="G118">
+      <c r="G118" s="7">
         <v>72</v>
       </c>
       <c r="H118">
@@ -44114,10 +44117,10 @@
       <c r="E119" t="s">
         <v>239</v>
       </c>
-      <c r="F119">
+      <c r="F119" s="7">
         <v>17</v>
       </c>
-      <c r="G119">
+      <c r="G119" s="7">
         <v>2.5</v>
       </c>
       <c r="H119">
@@ -44140,10 +44143,10 @@
       <c r="E120" t="s">
         <v>239</v>
       </c>
-      <c r="F120">
+      <c r="F120" s="7">
         <v>22</v>
       </c>
-      <c r="G120">
+      <c r="G120" s="7">
         <v>26</v>
       </c>
       <c r="H120">
@@ -44166,10 +44169,10 @@
       <c r="E121" t="s">
         <v>239</v>
       </c>
-      <c r="F121">
+      <c r="F121" s="7">
         <v>118</v>
       </c>
-      <c r="G121">
+      <c r="G121" s="7">
         <v>26</v>
       </c>
       <c r="H121">
@@ -44192,10 +44195,10 @@
       <c r="E122" t="s">
         <v>239</v>
       </c>
-      <c r="F122">
+      <c r="F122" s="7">
         <v>194</v>
       </c>
-      <c r="G122">
+      <c r="G122" s="7">
         <v>26</v>
       </c>
       <c r="H122">
@@ -44218,10 +44221,10 @@
       <c r="E123" t="s">
         <v>239</v>
       </c>
-      <c r="F123">
+      <c r="F123" s="7">
         <v>252</v>
       </c>
-      <c r="G123">
+      <c r="G123" s="7">
         <v>26</v>
       </c>
       <c r="H123">
@@ -44244,10 +44247,10 @@
       <c r="E124" t="s">
         <v>239</v>
       </c>
-      <c r="F124">
+      <c r="F124" s="7">
         <v>153</v>
       </c>
-      <c r="G124">
+      <c r="G124" s="7">
         <v>55</v>
       </c>
       <c r="H124">
@@ -44270,10 +44273,10 @@
       <c r="E125" t="s">
         <v>239</v>
       </c>
-      <c r="F125">
+      <c r="F125" s="7">
         <v>52</v>
       </c>
-      <c r="G125">
+      <c r="G125" s="7">
         <v>55</v>
       </c>
       <c r="H125">
@@ -44296,10 +44299,10 @@
       <c r="E126" t="s">
         <v>239</v>
       </c>
-      <c r="F126">
+      <c r="F126" s="7">
         <v>54</v>
       </c>
-      <c r="G126">
+      <c r="G126" s="7">
         <v>7.6</v>
       </c>
       <c r="H126">
@@ -44322,10 +44325,10 @@
       <c r="E127" t="s">
         <v>239</v>
       </c>
-      <c r="F127">
+      <c r="F127" s="7">
         <v>36</v>
       </c>
-      <c r="G127">
+      <c r="G127" s="7">
         <v>7.6</v>
       </c>
       <c r="H127">
@@ -44348,10 +44351,10 @@
       <c r="E128" t="s">
         <v>239</v>
       </c>
-      <c r="F128">
+      <c r="F128" s="7">
         <v>30</v>
       </c>
-      <c r="G128">
+      <c r="G128" s="7">
         <v>22</v>
       </c>
       <c r="H128">
@@ -44374,10 +44377,10 @@
       <c r="E129" t="s">
         <v>239</v>
       </c>
-      <c r="F129">
+      <c r="F129" s="7">
         <v>37</v>
       </c>
-      <c r="G129">
+      <c r="G129" s="7">
         <v>22</v>
       </c>
       <c r="H129">
@@ -44400,10 +44403,10 @@
       <c r="E130" t="s">
         <v>239</v>
       </c>
-      <c r="F130">
+      <c r="F130" s="7">
         <v>159</v>
       </c>
-      <c r="G130">
+      <c r="G130" s="7">
         <v>44</v>
       </c>
       <c r="H130">
@@ -44429,10 +44432,10 @@
       <c r="E131" t="s">
         <v>239</v>
       </c>
-      <c r="F131">
+      <c r="F131" s="7">
         <v>25</v>
       </c>
-      <c r="G131">
+      <c r="G131" s="7">
         <v>4.2</v>
       </c>
       <c r="H131">
@@ -44458,10 +44461,10 @@
       <c r="E132" t="s">
         <v>239</v>
       </c>
-      <c r="F132">
+      <c r="F132" s="7">
         <v>8</v>
       </c>
-      <c r="G132">
+      <c r="G132" s="7">
         <v>62</v>
       </c>
       <c r="H132">
@@ -44499,10 +44502,10 @@
       <c r="E133" t="s">
         <v>239</v>
       </c>
-      <c r="F133">
+      <c r="F133" s="7">
         <v>32</v>
       </c>
-      <c r="G133">
+      <c r="G133" s="7">
         <v>62</v>
       </c>
       <c r="H133">
@@ -44540,10 +44543,10 @@
       <c r="E134" t="s">
         <v>239</v>
       </c>
-      <c r="F134">
+      <c r="F134" s="7">
         <v>600</v>
       </c>
-      <c r="G134">
+      <c r="G134" s="7">
         <v>576</v>
       </c>
       <c r="H134">
@@ -44572,10 +44575,10 @@
       <c r="E135" t="s">
         <v>239</v>
       </c>
-      <c r="F135">
+      <c r="F135" s="7">
         <v>495</v>
       </c>
-      <c r="G135">
+      <c r="G135" s="7">
         <v>576</v>
       </c>
       <c r="H135">
@@ -44604,10 +44607,10 @@
       <c r="E136" t="s">
         <v>239</v>
       </c>
-      <c r="F136">
+      <c r="F136" s="7">
         <v>633</v>
       </c>
-      <c r="G136">
+      <c r="G136" s="7">
         <v>576</v>
       </c>
       <c r="H136">
@@ -44636,10 +44639,10 @@
       <c r="E137" t="s">
         <v>239</v>
       </c>
-      <c r="F137">
+      <c r="F137" s="7">
         <v>927</v>
       </c>
-      <c r="G137">
+      <c r="G137" s="7">
         <v>576</v>
       </c>
       <c r="H137">
@@ -44668,10 +44671,10 @@
       <c r="E138" t="s">
         <v>239</v>
       </c>
-      <c r="F138">
+      <c r="F138" s="7">
         <v>4210</v>
       </c>
-      <c r="G138">
+      <c r="G138" s="7">
         <v>576</v>
       </c>
       <c r="H138">
@@ -44700,10 +44703,10 @@
       <c r="E139" t="s">
         <v>239</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="7">
         <v>48</v>
       </c>
-      <c r="G139">
+      <c r="G139" s="7">
         <v>197</v>
       </c>
       <c r="H139">
@@ -44732,10 +44735,10 @@
       <c r="E140" t="s">
         <v>239</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="7">
         <v>87</v>
       </c>
-      <c r="G140">
+      <c r="G140" s="7">
         <v>197</v>
       </c>
       <c r="H140">
@@ -44764,10 +44767,10 @@
       <c r="E141" t="s">
         <v>239</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="7">
         <v>157</v>
       </c>
-      <c r="G141">
+      <c r="G141" s="7">
         <v>197</v>
       </c>
       <c r="H141">
@@ -44796,10 +44799,10 @@
       <c r="E142" t="s">
         <v>239</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="7">
         <v>138</v>
       </c>
-      <c r="G142">
+      <c r="G142" s="7">
         <v>197</v>
       </c>
       <c r="H142">
@@ -44828,10 +44831,10 @@
       <c r="E143" t="s">
         <v>239</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="7">
         <v>116</v>
       </c>
-      <c r="G143">
+      <c r="G143" s="7">
         <v>197</v>
       </c>
       <c r="H143">
@@ -44857,10 +44860,10 @@
       <c r="E144" t="s">
         <v>239</v>
       </c>
-      <c r="F144">
+      <c r="F144" s="7">
         <v>173</v>
       </c>
-      <c r="G144">
+      <c r="G144" s="7">
         <v>197</v>
       </c>
       <c r="H144">
@@ -44889,10 +44892,10 @@
       <c r="E145" t="s">
         <v>239</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="7">
         <v>173</v>
       </c>
-      <c r="G145">
+      <c r="G145" s="7">
         <v>1000</v>
       </c>
       <c r="H145">
@@ -44921,10 +44924,10 @@
       <c r="E146" t="s">
         <v>239</v>
       </c>
-      <c r="F146">
+      <c r="F146" s="7">
         <v>148</v>
       </c>
-      <c r="G146">
+      <c r="G146" s="7">
         <v>1000</v>
       </c>
       <c r="H146">
@@ -44953,10 +44956,10 @@
       <c r="E147" t="s">
         <v>239</v>
       </c>
-      <c r="F147">
+      <c r="F147" s="7">
         <v>28</v>
       </c>
-      <c r="G147">
+      <c r="G147" s="7">
         <v>275</v>
       </c>
       <c r="H147">
@@ -44985,10 +44988,10 @@
       <c r="E148" t="s">
         <v>239</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="7">
         <v>541</v>
       </c>
-      <c r="G148">
+      <c r="G148" s="7">
         <v>904</v>
       </c>
       <c r="H148">
@@ -45017,10 +45020,10 @@
       <c r="E149" t="s">
         <v>239</v>
       </c>
-      <c r="F149">
+      <c r="F149" s="7">
         <v>521</v>
       </c>
-      <c r="G149">
+      <c r="G149" s="7">
         <v>1230</v>
       </c>
       <c r="H149">
@@ -45049,10 +45052,10 @@
       <c r="E150" t="s">
         <v>239</v>
       </c>
-      <c r="F150">
+      <c r="F150" s="7">
         <v>493</v>
       </c>
-      <c r="G150">
+      <c r="G150" s="7">
         <v>1230</v>
       </c>
       <c r="H150">
@@ -45081,10 +45084,10 @@
       <c r="E151" t="s">
         <v>239</v>
       </c>
-      <c r="F151">
+      <c r="F151" s="7">
         <v>426</v>
       </c>
-      <c r="G151">
+      <c r="G151" s="7">
         <v>1230</v>
       </c>
       <c r="H151">
@@ -45113,10 +45116,10 @@
       <c r="E152" t="s">
         <v>239</v>
       </c>
-      <c r="F152">
+      <c r="F152" s="7">
         <v>738</v>
       </c>
-      <c r="G152">
+      <c r="G152" s="7">
         <v>1230</v>
       </c>
       <c r="H152">
@@ -45145,10 +45148,10 @@
       <c r="E153" t="s">
         <v>239</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="7">
         <v>382</v>
       </c>
-      <c r="G153">
+      <c r="G153" s="7">
         <v>1230</v>
       </c>
       <c r="H153">
@@ -45177,10 +45180,10 @@
       <c r="E154" t="s">
         <v>239</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="7">
         <v>267</v>
       </c>
-      <c r="G154">
+      <c r="G154" s="7">
         <v>1230</v>
       </c>
       <c r="H154">
@@ -45209,10 +45212,10 @@
       <c r="E155" t="s">
         <v>239</v>
       </c>
-      <c r="F155">
+      <c r="F155" s="7">
         <v>76</v>
       </c>
-      <c r="G155">
+      <c r="G155" s="7">
         <v>842</v>
       </c>
       <c r="H155">
@@ -45241,10 +45244,10 @@
       <c r="E156" t="s">
         <v>239</v>
       </c>
-      <c r="F156">
+      <c r="F156" s="7">
         <v>87</v>
       </c>
-      <c r="G156">
+      <c r="G156" s="7">
         <v>842</v>
       </c>
       <c r="H156">
@@ -45273,10 +45276,10 @@
       <c r="E157" t="s">
         <v>239</v>
       </c>
-      <c r="F157">
+      <c r="F157" s="7">
         <v>82</v>
       </c>
-      <c r="G157">
+      <c r="G157" s="7">
         <v>312</v>
       </c>
       <c r="H157">
@@ -45305,10 +45308,10 @@
       <c r="E158" t="s">
         <v>239</v>
       </c>
-      <c r="F158">
+      <c r="F158" s="7">
         <v>282</v>
       </c>
-      <c r="G158">
+      <c r="G158" s="7">
         <v>1620</v>
       </c>
       <c r="H158">
@@ -45337,10 +45340,10 @@
       <c r="E159" t="s">
         <v>239</v>
       </c>
-      <c r="F159">
+      <c r="F159" s="7">
         <v>123</v>
       </c>
-      <c r="G159">
+      <c r="G159" s="7">
         <v>1620</v>
       </c>
       <c r="H159">
@@ -45369,10 +45372,10 @@
       <c r="E160" t="s">
         <v>239</v>
       </c>
-      <c r="F160">
+      <c r="F160" s="7">
         <v>85</v>
       </c>
-      <c r="G160">
+      <c r="G160" s="7">
         <v>1620</v>
       </c>
       <c r="H160">
@@ -45401,10 +45404,10 @@
       <c r="E161" t="s">
         <v>239</v>
       </c>
-      <c r="F161">
+      <c r="F161" s="7">
         <v>215</v>
       </c>
-      <c r="G161">
+      <c r="G161" s="7">
         <v>1620</v>
       </c>
       <c r="H161">
@@ -45433,10 +45436,10 @@
       <c r="E162" t="s">
         <v>239</v>
       </c>
-      <c r="F162">
+      <c r="F162" s="7">
         <v>13</v>
       </c>
-      <c r="G162">
+      <c r="G162" s="7">
         <v>102</v>
       </c>
       <c r="H162">
@@ -45465,10 +45468,10 @@
       <c r="E163" t="s">
         <v>239</v>
       </c>
-      <c r="F163">
+      <c r="F163" s="7">
         <v>7</v>
       </c>
-      <c r="G163">
+      <c r="G163" s="7">
         <v>102</v>
       </c>
       <c r="H163">
@@ -45497,10 +45500,10 @@
       <c r="E164" t="s">
         <v>239</v>
       </c>
-      <c r="F164">
+      <c r="F164" s="7">
         <v>7</v>
       </c>
-      <c r="G164">
+      <c r="G164" s="7">
         <v>102</v>
       </c>
       <c r="H164">
@@ -45529,10 +45532,10 @@
       <c r="E165" t="s">
         <v>239</v>
       </c>
-      <c r="F165">
+      <c r="F165" s="7">
         <v>6</v>
       </c>
-      <c r="G165">
+      <c r="G165" s="7">
         <v>102</v>
       </c>
       <c r="H165">
@@ -45561,10 +45564,10 @@
       <c r="E166" t="s">
         <v>239</v>
       </c>
-      <c r="F166">
+      <c r="F166" s="7">
         <v>726</v>
       </c>
-      <c r="G166">
+      <c r="G166" s="7">
         <v>50</v>
       </c>
       <c r="H166">
@@ -45590,10 +45593,10 @@
       <c r="E167" t="s">
         <v>239</v>
       </c>
-      <c r="F167">
+      <c r="F167" s="7">
         <v>455</v>
       </c>
-      <c r="G167">
+      <c r="G167" s="7">
         <v>50</v>
       </c>
       <c r="H167">
@@ -45619,10 +45622,10 @@
       <c r="E168" t="s">
         <v>239</v>
       </c>
-      <c r="F168">
+      <c r="F168" s="7">
         <v>12</v>
       </c>
-      <c r="G168">
+      <c r="G168" s="7">
         <v>3.6</v>
       </c>
       <c r="H168">
@@ -45648,10 +45651,10 @@
       <c r="E169" t="s">
         <v>239</v>
       </c>
-      <c r="F169">
+      <c r="F169" s="7">
         <v>37</v>
       </c>
-      <c r="G169">
+      <c r="G169" s="7">
         <v>3.6</v>
       </c>
       <c r="H169">
@@ -45677,10 +45680,10 @@
       <c r="E170" t="s">
         <v>132</v>
       </c>
-      <c r="F170">
+      <c r="F170" s="7">
         <v>42</v>
       </c>
-      <c r="G170">
+      <c r="G170" s="7">
         <v>20</v>
       </c>
       <c r="H170">
@@ -45715,10 +45718,10 @@
       <c r="E171" t="s">
         <v>132</v>
       </c>
-      <c r="F171">
+      <c r="F171" s="7">
         <v>16</v>
       </c>
-      <c r="G171">
+      <c r="G171" s="7">
         <v>45</v>
       </c>
       <c r="H171">
@@ -45753,10 +45756,10 @@
       <c r="E172" t="s">
         <v>239</v>
       </c>
-      <c r="F172">
+      <c r="F172" s="7">
         <v>6</v>
       </c>
-      <c r="G172">
+      <c r="G172" s="7">
         <v>0.37</v>
       </c>
       <c r="H172">
@@ -45791,10 +45794,10 @@
       <c r="E173" t="s">
         <v>239</v>
       </c>
-      <c r="F173">
+      <c r="F173" s="7">
         <v>352</v>
       </c>
-      <c r="G173">
+      <c r="G173" s="7">
         <v>217</v>
       </c>
       <c r="H173">
@@ -45829,10 +45832,10 @@
       <c r="E174" t="s">
         <v>239</v>
       </c>
-      <c r="F174">
+      <c r="F174" s="7">
         <v>163</v>
       </c>
-      <c r="G174">
+      <c r="G174" s="7">
         <v>217</v>
       </c>
       <c r="H174">
@@ -45867,10 +45870,10 @@
       <c r="E175" t="s">
         <v>239</v>
       </c>
-      <c r="F175">
+      <c r="F175" s="7">
         <v>373</v>
       </c>
-      <c r="G175">
+      <c r="G175" s="7">
         <v>1500</v>
       </c>
       <c r="H175">
@@ -45905,10 +45908,10 @@
       <c r="E176" t="s">
         <v>239</v>
       </c>
-      <c r="F176">
+      <c r="F176" s="7">
         <v>823</v>
       </c>
-      <c r="G176">
+      <c r="G176" s="7">
         <v>1500</v>
       </c>
       <c r="H176">
@@ -45943,10 +45946,10 @@
       <c r="E177" t="s">
         <v>239</v>
       </c>
-      <c r="F177">
+      <c r="F177" s="7">
         <v>689</v>
       </c>
-      <c r="G177">
+      <c r="G177" s="7">
         <v>1500</v>
       </c>
       <c r="H177">
@@ -45981,10 +45984,10 @@
       <c r="E178" t="s">
         <v>239</v>
       </c>
-      <c r="F178">
+      <c r="F178" s="7">
         <v>335</v>
       </c>
-      <c r="G178">
+      <c r="G178" s="7">
         <v>1500</v>
       </c>
       <c r="H178">
@@ -46022,10 +46025,10 @@
       <c r="E179" t="s">
         <v>239</v>
       </c>
-      <c r="F179">
+      <c r="F179" s="7">
         <v>135</v>
       </c>
-      <c r="G179">
+      <c r="G179" s="7">
         <v>1500</v>
       </c>
       <c r="H179">
@@ -46060,10 +46063,10 @@
       <c r="E180" t="s">
         <v>239</v>
       </c>
-      <c r="F180">
+      <c r="F180" s="7">
         <v>34</v>
       </c>
-      <c r="G180">
+      <c r="G180" s="7">
         <v>183</v>
       </c>
       <c r="H180">
@@ -46098,10 +46101,10 @@
       <c r="E181" t="s">
         <v>239</v>
       </c>
-      <c r="F181">
+      <c r="F181" s="7">
         <v>28</v>
       </c>
-      <c r="G181">
+      <c r="G181" s="7">
         <v>183</v>
       </c>
       <c r="H181">
@@ -46136,10 +46139,10 @@
       <c r="E182" t="s">
         <v>239</v>
       </c>
-      <c r="F182">
+      <c r="F182" s="7">
         <v>28</v>
       </c>
-      <c r="G182">
+      <c r="G182" s="7">
         <v>183</v>
       </c>
       <c r="H182">
@@ -46174,9 +46177,10 @@
       <c r="E183" t="s">
         <v>239</v>
       </c>
-      <c r="F183">
+      <c r="F183" s="7">
         <v>99</v>
       </c>
+      <c r="G183" s="6"/>
       <c r="O183">
         <v>97</v>
       </c>
@@ -46209,9 +46213,10 @@
       <c r="E184" t="s">
         <v>239</v>
       </c>
-      <c r="F184">
+      <c r="F184" s="7">
         <v>186</v>
       </c>
+      <c r="G184" s="6"/>
       <c r="O184">
         <v>99</v>
       </c>
@@ -46244,9 +46249,10 @@
       <c r="E185" t="s">
         <v>239</v>
       </c>
-      <c r="F185">
+      <c r="F185" s="7">
         <v>1010</v>
       </c>
+      <c r="G185" s="6"/>
       <c r="O185">
         <v>97</v>
       </c>
@@ -46279,9 +46285,10 @@
       <c r="E186" t="s">
         <v>239</v>
       </c>
-      <c r="F186">
+      <c r="F186" s="7">
         <v>256</v>
       </c>
+      <c r="G186" s="6"/>
       <c r="O186">
         <v>89</v>
       </c>
@@ -46314,9 +46321,10 @@
       <c r="E187" t="s">
         <v>239</v>
       </c>
-      <c r="F187">
+      <c r="F187" s="7">
         <v>237</v>
       </c>
+      <c r="G187" s="6"/>
       <c r="O187">
         <v>89</v>
       </c>
@@ -46349,9 +46357,10 @@
       <c r="E188" t="s">
         <v>239</v>
       </c>
-      <c r="F188">
+      <c r="F188" s="7">
         <v>231</v>
       </c>
+      <c r="G188" s="6"/>
       <c r="O188">
         <v>89</v>
       </c>
@@ -46384,9 +46393,10 @@
       <c r="E189" t="s">
         <v>239</v>
       </c>
-      <c r="F189">
+      <c r="F189" s="7">
         <v>195</v>
       </c>
+      <c r="G189" s="6"/>
       <c r="O189">
         <v>92</v>
       </c>
@@ -46419,9 +46429,10 @@
       <c r="E190" t="s">
         <v>239</v>
       </c>
-      <c r="F190">
+      <c r="F190" s="7">
         <v>115</v>
       </c>
+      <c r="G190" s="6"/>
       <c r="O190">
         <v>91</v>
       </c>
@@ -46454,9 +46465,10 @@
       <c r="E191" t="s">
         <v>239</v>
       </c>
-      <c r="F191">
+      <c r="F191" s="7">
         <v>100</v>
       </c>
+      <c r="G191" s="6"/>
       <c r="O191">
         <v>96</v>
       </c>
@@ -46489,9 +46501,10 @@
       <c r="E192" t="s">
         <v>239</v>
       </c>
-      <c r="F192">
+      <c r="F192" s="7">
         <v>100</v>
       </c>
+      <c r="G192" s="6"/>
       <c r="O192">
         <v>97</v>
       </c>
@@ -46524,9 +46537,10 @@
       <c r="E193" t="s">
         <v>239</v>
       </c>
-      <c r="F193">
+      <c r="F193" s="7">
         <v>82</v>
       </c>
+      <c r="G193" s="6"/>
       <c r="O193">
         <v>97</v>
       </c>
@@ -46559,9 +46573,10 @@
       <c r="E194" t="s">
         <v>239</v>
       </c>
-      <c r="F194">
-        <v>9</v>
-      </c>
+      <c r="F194" s="7">
+        <v>9</v>
+      </c>
+      <c r="G194" s="6"/>
       <c r="Y194">
         <v>70</v>
       </c>
@@ -46588,9 +46603,10 @@
       <c r="E195" t="s">
         <v>239</v>
       </c>
-      <c r="F195">
+      <c r="F195" s="7">
         <v>16</v>
       </c>
+      <c r="G195" s="6"/>
       <c r="Y195">
         <v>70</v>
       </c>

</xml_diff>